<commit_message>
Excel filling with data done. Seperation on relation
</commit_message>
<xml_diff>
--- a/src/AppBundle/Factory/excel/overzicht btw.xlsx
+++ b/src/AppBundle/Factory/excel/overzicht btw.xlsx
@@ -167,7 +167,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,10 +202,6 @@
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -261,7 +257,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,9 +379,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="8" t="n">
         <v>0</v>
       </c>
@@ -397,7 +392,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="D13" s="8" t="n">
         <v>0</v>
       </c>
@@ -409,7 +404,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="D14" s="8" t="n">
         <v>0</v>
       </c>
@@ -421,7 +416,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="D15" s="8" t="n">
         <v>0</v>
       </c>
@@ -433,7 +428,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="D16" s="8" t="n">
         <v>0</v>
       </c>
@@ -445,7 +440,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="D17" s="8" t="n">
         <v>0</v>
       </c>
@@ -457,7 +452,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="D18" s="8" t="n">
         <v>0</v>
       </c>
@@ -469,7 +464,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="D19" s="8" t="n">
         <v>0</v>
       </c>
@@ -491,15 +486,15 @@
         <v>10</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="D21" s="13" t="n">
+      <c r="D21" s="12" t="n">
         <f aca="false">SUM(D6:D20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="13" t="n">
+      <c r="E21" s="12" t="n">
         <f aca="false">SUM(E6:E20)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="13" t="n">
+      <c r="F21" s="12" t="n">
         <f aca="false">SUM(F6:F20)</f>
         <v>0</v>
       </c>
@@ -526,7 +521,7 @@
       <c r="A27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -591,9 +586,9 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="8" t="n">
         <v>0</v>
       </c>
@@ -606,8 +601,8 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="8" t="n">
         <v>0</v>
       </c>
@@ -656,7 +651,7 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="C37" s="17"/>
+      <c r="C37" s="16"/>
       <c r="D37" s="8" t="n">
         <v>0</v>
       </c>
@@ -705,8 +700,8 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
       <c r="D41" s="8" t="n">
         <v>0</v>
       </c>
@@ -720,8 +715,8 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
       <c r="D42" s="8" t="n">
         <v>0</v>
       </c>
@@ -735,8 +730,8 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
       <c r="D43" s="8" t="n">
         <v>0</v>
       </c>
@@ -750,8 +745,8 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="17"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -761,15 +756,15 @@
         <v>10</v>
       </c>
       <c r="B45" s="7"/>
-      <c r="D45" s="13" t="n">
+      <c r="D45" s="12" t="n">
         <f aca="false">SUM(D28:D44)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="13" t="n">
+      <c r="E45" s="12" t="n">
         <f aca="false">SUM(E28:E44)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="13" t="n">
+      <c r="F45" s="12" t="n">
         <f aca="false">SUM(F28:F44)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
deviding invoices on relations. New way to write cellValue
</commit_message>
<xml_diff>
--- a/src/AppBundle/Factory/excel/overzicht btw.xlsx
+++ b/src/AppBundle/Factory/excel/overzicht btw.xlsx
@@ -167,7 +167,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,6 +204,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -224,8 +228,24 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -257,7 +277,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -326,7 +346,7 @@
       <c r="E7" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -338,7 +358,7 @@
       <c r="E8" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -350,7 +370,7 @@
       <c r="E9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -362,7 +382,7 @@
       <c r="E10" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -374,104 +394,104 @@
       <c r="E11" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="11"/>
+      <c r="B13" s="12"/>
       <c r="D13" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="11"/>
+      <c r="B14" s="12"/>
       <c r="D14" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="11"/>
+      <c r="B15" s="12"/>
       <c r="D15" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E15" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="11"/>
+      <c r="B16" s="12"/>
       <c r="D16" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="11"/>
+      <c r="B17" s="12"/>
       <c r="D17" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="8" t="n">
+      <c r="F17" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="11"/>
+      <c r="B18" s="12"/>
       <c r="D18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F18" s="8" t="n">
+      <c r="F18" s="9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="11"/>
+      <c r="B19" s="12"/>
       <c r="D19" s="8" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="F19" s="8" t="n">
+      <c r="F19" s="9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -486,15 +506,15 @@
         <v>10</v>
       </c>
       <c r="B21" s="7"/>
-      <c r="D21" s="12" t="n">
+      <c r="D21" s="13" t="n">
         <f aca="false">SUM(D6:D20)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="12" t="n">
+      <c r="E21" s="13" t="n">
         <f aca="false">SUM(E6:E20)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="12" t="n">
+      <c r="F21" s="13" t="n">
         <f aca="false">SUM(F6:F20)</f>
         <v>0</v>
       </c>
@@ -521,7 +541,7 @@
       <c r="A27" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -544,7 +564,9 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="7"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="8" t="n">
         <v>0</v>
       </c>
@@ -558,7 +580,8 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="8" t="n">
         <v>0</v>
       </c>
@@ -571,9 +594,9 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="A31" s="17"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="8" t="n">
         <v>0</v>
       </c>
@@ -586,9 +609,9 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="8" t="n">
         <v>0</v>
       </c>
@@ -601,8 +624,8 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="8" t="n">
         <v>0</v>
       </c>
@@ -615,6 +638,8 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="8" t="n">
         <v>0</v>
       </c>
@@ -627,6 +652,8 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
       <c r="D35" s="8" t="n">
         <v>0</v>
       </c>
@@ -639,6 +666,8 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
       <c r="D36" s="8" t="n">
         <v>0</v>
       </c>
@@ -651,7 +680,8 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
-      <c r="C37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="8" t="n">
         <v>0</v>
       </c>
@@ -664,6 +694,8 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="8" t="n">
         <v>0</v>
       </c>
@@ -676,6 +708,8 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
+      <c r="B39" s="16"/>
+      <c r="C39" s="16"/>
       <c r="D39" s="8" t="n">
         <v>0</v>
       </c>
@@ -688,6 +722,8 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
       <c r="D40" s="8" t="n">
         <v>0</v>
       </c>
@@ -700,8 +736,8 @@
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="8" t="n">
         <v>0</v>
       </c>
@@ -715,8 +751,8 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="16"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="8" t="n">
         <v>0</v>
       </c>
@@ -730,8 +766,8 @@
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="16"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="8" t="n">
         <v>0</v>
       </c>
@@ -745,8 +781,8 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="5"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="16"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
@@ -756,15 +792,15 @@
         <v>10</v>
       </c>
       <c r="B45" s="7"/>
-      <c r="D45" s="12" t="n">
+      <c r="D45" s="13" t="n">
         <f aca="false">SUM(D28:D44)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="12" t="n">
+      <c r="E45" s="13" t="n">
         <f aca="false">SUM(E28:E44)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="12" t="n">
+      <c r="F45" s="13" t="n">
         <f aca="false">SUM(F28:F44)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
contactform and shade on indexes
</commit_message>
<xml_diff>
--- a/src/AppBundle/Factory/excel/overzicht btw.xlsx
+++ b/src/AppBundle/Factory/excel/overzicht btw.xlsx
@@ -276,8 +276,8 @@
   </sheetPr>
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>